<commit_message>
Completed the Stimmelmayr and Arnold datasets. Read in the LTEMP and Ma datasets.
</commit_message>
<xml_diff>
--- a/Input Data/Stimmelmayr et al 2018_Seal_MinedTable4.xlsx
+++ b/Input Data/Stimmelmayr et al 2018_Seal_MinedTable4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Tributary Research Consulting LLC\Contracts and Jobs\2025\FFS (M. Bender) GIS mapping\OSRI_Alaska_Food_Contamination\Input Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EACDA99-9831-D14D-B847-7025C937F6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFF705A-8340-41D6-B551-78F75C64A7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{2143D6EE-5463-2C4D-B572-B52F1427B616}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2143D6EE-5463-2C4D-B572-B52F1427B616}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -643,19 +643,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54ADE886-64B1-DF4F-BE69-6282EB85B64E}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="4"/>
-    <col min="19" max="19" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="3" max="3" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="4"/>
+    <col min="19" max="19" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -668,7 +669,7 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F1" t="s">
@@ -717,7 +718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -776,7 +777,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -835,7 +836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -897,7 +898,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -959,7 +960,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -972,7 +973,7 @@
       <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1016,7 +1017,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1255,7 +1256,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1445,7 +1446,7 @@
       <c r="D14" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -1489,7 +1490,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1735,7 +1736,7 @@
       <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1779,7 +1780,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1960,7 +1961,7 @@
       <c r="D23" t="s">
         <v>36</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -2004,7 +2005,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -2066,7 +2067,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2380,7 +2381,7 @@
       <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -2424,7 +2425,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2483,25 +2484,25 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
   </sheetData>

</xml_diff>